<commit_message>
Spreadsheet and fmod update
</commit_message>
<xml_diff>
--- a/Fmod/audio managment sheet.xlsx
+++ b/Fmod/audio managment sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Documents\Audio 4 Games\GameJam\BringTheBandBack\Fmod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\joshd\Documents\BringTheBandBack\Fmod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4098C880-6590-47DF-8707-AE4AFD3E353F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE36DB7-8704-4EE2-B7B3-30AAB7989D44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24795" yWindow="1800" windowWidth="23970" windowHeight="12720" xr2:uid="{9A0D5F0E-D7D4-4C8C-99E5-94DD75E2F993}"/>
+    <workbookView xWindow="12060" yWindow="225" windowWidth="7950" windowHeight="9675" xr2:uid="{9A0D5F0E-D7D4-4C8C-99E5-94DD75E2F993}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Event Path</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>CymbalContact</t>
+  </si>
+  <si>
+    <t>:/Atmos/Haunting</t>
+  </si>
+  <si>
+    <t>:/Drums/StickCollison</t>
+  </si>
+  <si>
+    <t>StickCollision</t>
   </si>
 </sst>
 </file>
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69FDC269-D59F-4971-B506-002CE6DCBEA9}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +632,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -632,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
@@ -643,44 +652,50 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -695,7 +710,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
@@ -710,7 +725,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
@@ -725,7 +740,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
@@ -740,75 +755,105 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>